<commit_message>
delay laitettu että muokkaus menee helpommin
</commit_message>
<xml_diff>
--- a/Laskupohja.xlsx
+++ b/Laskupohja.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" checkCompatibility="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6149C233-5316-4886-BD61-5CC4372CB8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE73FE7-58BD-4F28-B39F-3326E01433B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="24" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>INVOICE</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>nikolettberkinevarga@gmail.com</t>
-  </si>
-  <si>
-    <t>Juustokakku 12 hlö</t>
   </si>
   <si>
     <t>19.09.2025</t>
@@ -1356,8 +1353,8 @@
   </sheetPr>
   <dimension ref="B1:F44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,14 +1416,14 @@
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="13">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1482,7 @@
     </row>
     <row r="16" spans="2:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="27">
         <v>1</v>
@@ -1500,7 +1497,7 @@
     </row>
     <row r="17" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="30">
         <v>1</v>
@@ -1514,18 +1511,12 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="30">
-        <v>1</v>
-      </c>
-      <c r="D18" s="31">
-        <v>48.5</v>
-      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="32">
         <f t="shared" si="0"/>
-        <v>48.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1646,7 +1637,7 @@
       <c r="D31" s="50"/>
       <c r="E31" s="35">
         <f>SUM(E16:E29)</f>
-        <v>168.5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1667,7 +1658,7 @@
       <c r="D33" s="20"/>
       <c r="E33" s="35">
         <f>ROUND(E31 * ($E$32/(1+$E$32)), 2)</f>
-        <v>32.61</v>
+        <v>23.23</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,7 +1669,7 @@
       <c r="D34" s="42"/>
       <c r="E34" s="47">
         <f>E31</f>
-        <v>168.5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>